<commit_message>
simulation summary metrics localization entries added
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.RICK\Desktop\it-alert-newclone\Unity\Assets\Editor\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\it-alert\Unity\Assets\Editor\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49DBDBCF-0C67-4C80-8BD5-D7A1BB434DD8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E79C3877-6482-42CE-A699-E5060926A7CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="296">
   <si>
     <t>Key</t>
   </si>
@@ -811,7 +811,103 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>Overzicht</t>
+    <t>SIMULATION_SUMMARY_METRIC_SPOKE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_MOVED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_SENT</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_RECEIVED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVURUSES_USED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANNERS_USED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_KILLED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_WASTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANS_WITH_NO_VIRUSES_FOUND</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURES_USED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_CAPTURED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURE_WITH_NO_VIRUS_CAUGHT</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANALYSERS_USED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATED</t>
+  </si>
+  <si>
+    <t>Spoke</t>
+  </si>
+  <si>
+    <t>Moved</t>
+  </si>
+  <si>
+    <t>Transfers Received</t>
+  </si>
+  <si>
+    <t>Transfers Sent</t>
+  </si>
+  <si>
+    <t>Antiviruses Used</t>
+  </si>
+  <si>
+    <t>Scanners Used</t>
+  </si>
+  <si>
+    <t>Viruses Killed</t>
+  </si>
+  <si>
+    <t>Antiviruses Wasted</t>
+  </si>
+  <si>
+    <t>Viruses Found</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_FOUND</t>
+  </si>
+  <si>
+    <t>Scans w/o Viruses Found</t>
+  </si>
+  <si>
+    <t>Capture w/o Virus Caught</t>
+  </si>
+  <si>
+    <t>Captures Used</t>
+  </si>
+  <si>
+    <t>Viruses Captured</t>
+  </si>
+  <si>
+    <t>Analysers Used</t>
+  </si>
+  <si>
+    <t>Antiviruses Created</t>
+  </si>
+  <si>
+    <t>Antivirus Creation Fails</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATION_FAILS</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
   </si>
 </sst>
 </file>
@@ -893,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -912,6 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1252,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2460,7 +2557,7 @@
         <v>262</v>
       </c>
       <c r="C96" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -2470,99 +2567,229 @@
       <c r="B97" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C97" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25"/>
+      <c r="C97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>263</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C98" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
+      <c r="A99" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C99" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
+      <c r="A100" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
+      <c r="A101" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C101" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
+      <c r="A102" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C102" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
+      <c r="A103" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C103" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
+      <c r="A104" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C104" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
+      <c r="A105" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C105" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
+      <c r="A106" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C106" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="12"/>
+      <c r="A107" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C107" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
+      <c r="A108" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C108" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
+      <c r="A109" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C109" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
+      <c r="A110" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C110" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
+      <c r="A111" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C111" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-    </row>
-    <row r="113" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-    </row>
-    <row r="114" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C112" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C113" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
     </row>
-    <row r="119" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
     </row>
-    <row r="120" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
     </row>
-    <row r="121" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
     </row>
-    <row r="122" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
     </row>
-    <row r="123" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
     </row>
-    <row r="124" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
     </row>
-    <row r="125" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
     </row>
-    <row r="126" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
     </row>
-    <row r="127" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
     </row>
-    <row r="128" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
     </row>
     <row r="129" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add translations for metric titles and descriptions
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\it-alert\Unity\Assets\Editor\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\ITALERTTEST\Unity\Assets\Editor\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E79C3877-6482-42CE-A699-E5060926A7CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960"/>
   </bookViews>
   <sheets>
     <sheet name="UILocalizations" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="360">
   <si>
     <t>Key</t>
   </si>
@@ -908,12 +907,204 @@
   </si>
   <si>
     <t>xxxxx</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SPOKE_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SPOKE_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_MOVED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_MOVED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_SENT_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_SENT_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_RECEIVED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVURUSES_USED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANNERS_USED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_KILLED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_WASTED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_FOUND_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANS_WITH_NO_VIRUSES_FOUND_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURES_USED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_CAPTURED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURE_WITH_NO_VIRUS_CAUGHT_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANALYSERS_USED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATED_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATION_FAILS_TITLE</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_RECEIVED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVURUSES_USED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANNERS_USED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_KILLED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_WASTED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_FOUND_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANS_WITH_NO_VIRUSES_FOUND_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURES_USED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_CAPTURED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURE_WITH_NO_VIRUS_CAUGHT_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANALYSERS_USED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATED_FORMATTED</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATION_FAILS_FORMATTED</t>
+  </si>
+  <si>
+    <t>Chatterbox</t>
+  </si>
+  <si>
+    <t>{0} Times Spoken</t>
+  </si>
+  <si>
+    <t>Traveller</t>
+  </si>
+  <si>
+    <t>{0} Nodes Moved</t>
+  </si>
+  <si>
+    <t>Uploader</t>
+  </si>
+  <si>
+    <t>{0} Transfers Sent</t>
+  </si>
+  <si>
+    <t>Downloader</t>
+  </si>
+  <si>
+    <t>{0} Transfers Received</t>
+  </si>
+  <si>
+    <t>Surgeon</t>
+  </si>
+  <si>
+    <t>{0} Antiviruses Used</t>
+  </si>
+  <si>
+    <t>Detective</t>
+  </si>
+  <si>
+    <t>{0} Scanners Used</t>
+  </si>
+  <si>
+    <t>Eliminator</t>
+  </si>
+  <si>
+    <t>{0} Viruses Removed</t>
+  </si>
+  <si>
+    <t>Spiller</t>
+  </si>
+  <si>
+    <t>{0} Antiviruses Wasted</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
+    <t>{0} Viruses Found</t>
+  </si>
+  <si>
+    <t>Phisher</t>
+  </si>
+  <si>
+    <t>{0} Times Scanned Without Virus</t>
+  </si>
+  <si>
+    <t>Bug Hunter</t>
+  </si>
+  <si>
+    <t>{0} Captures Used</t>
+  </si>
+  <si>
+    <t>Bug Catcher</t>
+  </si>
+  <si>
+    <t>{0} Viruses Captured</t>
+  </si>
+  <si>
+    <t>Bad Debugger</t>
+  </si>
+  <si>
+    <t>Scientist</t>
+  </si>
+  <si>
+    <t>{0} Analysers Used</t>
+  </si>
+  <si>
+    <t>Splicer</t>
+  </si>
+  <si>
+    <t>{0} Antiviruses Created</t>
+  </si>
+  <si>
+    <t>Failed to Capture {0} Times</t>
+  </si>
+  <si>
+    <t>Failed to Create Antivirus {0} Times</t>
+  </si>
+  <si>
+    <t>Blindfire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1102,23 +1293,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1154,23 +1328,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1346,16 +1503,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1002"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" customWidth="1"/>
+    <col min="1" max="1" width="94.36328125" customWidth="1"/>
     <col min="2" max="2" width="51.81640625" customWidth="1"/>
     <col min="3" max="3" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2583,44 +2740,44 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>278</v>
+      <c r="A99" t="s">
+        <v>296</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>328</v>
       </c>
       <c r="C99" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>280</v>
+      <c r="A100" t="s">
+        <v>297</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>329</v>
       </c>
       <c r="C100" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
-        <v>266</v>
+      <c r="A101" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C101" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
-        <v>267</v>
+      <c r="A102" s="13" t="s">
+        <v>298</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>281</v>
+        <v>330</v>
       </c>
       <c r="C102" t="s">
         <v>295</v>
@@ -2628,10 +2785,10 @@
     </row>
     <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>282</v>
+        <v>331</v>
       </c>
       <c r="C103" t="s">
         <v>295</v>
@@ -2639,21 +2796,21 @@
     </row>
     <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C104" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>270</v>
+      <c r="A105" s="13" t="s">
+        <v>300</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>284</v>
+        <v>332</v>
       </c>
       <c r="C105" t="s">
         <v>295</v>
@@ -2661,43 +2818,43 @@
     </row>
     <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>285</v>
+        <v>333</v>
       </c>
       <c r="C106" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>271</v>
+      <c r="A107" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C107" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>272</v>
+      <c r="A108" s="13" t="s">
+        <v>302</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>289</v>
+        <v>334</v>
       </c>
       <c r="C108" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
-        <v>273</v>
+      <c r="A109" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>290</v>
+        <v>335</v>
       </c>
       <c r="C109" t="s">
         <v>295</v>
@@ -2705,32 +2862,32 @@
     </row>
     <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C110" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
-        <v>275</v>
+      <c r="A111" s="13" t="s">
+        <v>303</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>291</v>
+        <v>336</v>
       </c>
       <c r="C111" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>276</v>
+      <c r="A112" s="13" t="s">
+        <v>316</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
       <c r="C112" t="s">
         <v>295</v>
@@ -2738,154 +2895,410 @@
     </row>
     <row r="113" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C113" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
+      <c r="A114" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C114" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
+      <c r="A115" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="C115" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="116" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
+      <c r="A116" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C116" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="117" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
+      <c r="A117" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="C117" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="118" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
+      <c r="A118" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="C118" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="119" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
+      <c r="A119" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C119" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="120" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
+      <c r="A120" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C120" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="121" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
+      <c r="A121" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="C121" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
+      <c r="A122" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C122" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
+      <c r="A123" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C123" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="124" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="12"/>
+      <c r="A124" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="C124" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="125" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
+      <c r="A125" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C125" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
+      <c r="A126" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C126" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="12"/>
+      <c r="A127" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C127" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="128" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="12"/>
-    </row>
-    <row r="129" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
-    </row>
-    <row r="130" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="12"/>
-    </row>
-    <row r="131" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="12"/>
-    </row>
-    <row r="132" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="12"/>
-    </row>
-    <row r="133" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A133" s="12"/>
-    </row>
-    <row r="134" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="12"/>
-    </row>
-    <row r="135" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="12"/>
-    </row>
-    <row r="136" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="12"/>
-    </row>
-    <row r="137" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="12"/>
-    </row>
-    <row r="138" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="12"/>
-    </row>
-    <row r="139" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="12"/>
-    </row>
-    <row r="140" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="12"/>
-    </row>
-    <row r="141" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="12"/>
-    </row>
-    <row r="142" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="12"/>
-    </row>
-    <row r="143" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="12"/>
-    </row>
-    <row r="144" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A144" s="12"/>
-    </row>
-    <row r="145" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="12"/>
-    </row>
-    <row r="146" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C128" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C129" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C130" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C131" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C132" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C133" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C134" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C135" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C136" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C137" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="C138" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C139" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C140" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C141" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C142" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C143" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C144" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C145" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
     </row>
-    <row r="147" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
     </row>
-    <row r="148" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
     </row>
-    <row r="149" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
     </row>
-    <row r="150" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
     </row>
-    <row r="151" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
     </row>
-    <row r="152" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
     </row>
-    <row r="153" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
     </row>
-    <row r="154" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
     </row>
-    <row r="155" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
     </row>
-    <row r="156" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
     </row>
-    <row r="157" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
     </row>
-    <row r="158" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
     </row>
-    <row r="159" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
     </row>
-    <row r="160" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
     </row>
     <row r="161" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
@@ -5413,6 +5826,96 @@
     </row>
     <row r="1002" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1002" s="12"/>
+    </row>
+    <row r="1003" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1003" s="12"/>
+    </row>
+    <row r="1004" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1004" s="12"/>
+    </row>
+    <row r="1005" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1005" s="12"/>
+    </row>
+    <row r="1006" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1006" s="12"/>
+    </row>
+    <row r="1007" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1007" s="12"/>
+    </row>
+    <row r="1008" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1008" s="12"/>
+    </row>
+    <row r="1009" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1009" s="12"/>
+    </row>
+    <row r="1010" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1010" s="12"/>
+    </row>
+    <row r="1011" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1011" s="12"/>
+    </row>
+    <row r="1012" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1012" s="12"/>
+    </row>
+    <row r="1013" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1013" s="12"/>
+    </row>
+    <row r="1014" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1014" s="12"/>
+    </row>
+    <row r="1015" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1015" s="12"/>
+    </row>
+    <row r="1016" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1016" s="12"/>
+    </row>
+    <row r="1017" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1017" s="12"/>
+    </row>
+    <row r="1018" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1018" s="12"/>
+    </row>
+    <row r="1019" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1019" s="12"/>
+    </row>
+    <row r="1020" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1020" s="12"/>
+    </row>
+    <row r="1021" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1021" s="12"/>
+    </row>
+    <row r="1022" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1022" s="12"/>
+    </row>
+    <row r="1023" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1023" s="12"/>
+    </row>
+    <row r="1024" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1024" s="12"/>
+    </row>
+    <row r="1025" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1025" s="12"/>
+    </row>
+    <row r="1026" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1026" s="12"/>
+    </row>
+    <row r="1027" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1027" s="12"/>
+    </row>
+    <row r="1028" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1028" s="12"/>
+    </row>
+    <row r="1029" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1029" s="12"/>
+    </row>
+    <row r="1030" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1030" s="12"/>
+    </row>
+    <row r="1031" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1031" s="12"/>
+    </row>
+    <row r="1032" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1032" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
set tests to use correct colours set player metric description back to include counts of actions
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="392">
   <si>
     <t>Key</t>
   </si>
@@ -1008,97 +1008,193 @@
     <t>Chatterbox</t>
   </si>
   <si>
-    <t>{0} Times Spoken</t>
-  </si>
-  <si>
     <t>Traveller</t>
   </si>
   <si>
-    <t>{0} Nodes Moved</t>
-  </si>
-  <si>
     <t>Uploader</t>
   </si>
   <si>
-    <t>{0} Transfers Sent</t>
-  </si>
-  <si>
     <t>Downloader</t>
   </si>
   <si>
-    <t>{0} Transfers Received</t>
-  </si>
-  <si>
     <t>Surgeon</t>
   </si>
   <si>
-    <t>{0} Antiviruses Used</t>
-  </si>
-  <si>
     <t>Detective</t>
   </si>
   <si>
-    <t>{0} Scanners Used</t>
-  </si>
-  <si>
     <t>Eliminator</t>
   </si>
   <si>
-    <t>{0} Viruses Removed</t>
-  </si>
-  <si>
     <t>Spiller</t>
   </si>
   <si>
-    <t>{0} Antiviruses Wasted</t>
-  </si>
-  <si>
     <t>Locator</t>
   </si>
   <si>
-    <t>{0} Viruses Found</t>
-  </si>
-  <si>
     <t>Phisher</t>
   </si>
   <si>
-    <t>{0} Times Scanned Without Virus</t>
-  </si>
-  <si>
     <t>Bug Hunter</t>
   </si>
   <si>
-    <t>{0} Captures Used</t>
-  </si>
-  <si>
     <t>Bug Catcher</t>
   </si>
   <si>
-    <t>{0} Viruses Captured</t>
-  </si>
-  <si>
     <t>Bad Debugger</t>
   </si>
   <si>
     <t>Scientist</t>
   </si>
   <si>
-    <t>{0} Analysers Used</t>
-  </si>
-  <si>
     <t>Splicer</t>
   </si>
   <si>
-    <t>{0} Antiviruses Created</t>
-  </si>
-  <si>
-    <t>Failed to Capture {0} Times</t>
-  </si>
-  <si>
-    <t>Failed to Create Antivirus {0} Times</t>
-  </si>
-  <si>
     <t>Blindfire</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SPOKE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Spoke Most Times</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_MOVED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Moved Most Nodes</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_SENT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Sent Most Items</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_TRANSFERS_RECEIVED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Received Most Items</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVURUSES_USED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Used Most Antivirus</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANNERS_USED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Used Most Scanners</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_KILLED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Removed Most Viruses</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_WASTED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Wasted Most Antivirus</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_FOUND_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Found Most Viruses</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_SCANS_WITH_NO_VIRUSES_FOUND_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURES_USED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Used Capture Most</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_VIRUSES_CAPTURED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Captured Most Viruses</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_CAPTURE_WITH_NO_VIRUS_CAUGHT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANALYSERS_USED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Most Analysers Used</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Created Most Antivirus</t>
+  </si>
+  <si>
+    <t>SIMULATION_SUMMARY_METRIC_ANTIVIRUSES_CREATION_FAILS_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Wasted Most Analyser Actions</t>
+  </si>
+  <si>
+    <t>Wasted Most Capture Actions</t>
+  </si>
+  <si>
+    <t>Wasted Most Scan Actions</t>
+  </si>
+  <si>
+    <t>Spoke {0} Times</t>
+  </si>
+  <si>
+    <t>Moved {0} Nodes</t>
+  </si>
+  <si>
+    <t>Sent {0} Transfers</t>
+  </si>
+  <si>
+    <t>Received {0} Transfers</t>
+  </si>
+  <si>
+    <t>Used {0} Antiviruses</t>
+  </si>
+  <si>
+    <t>Used {0} Scanners</t>
+  </si>
+  <si>
+    <t>Removed {0} Viruses</t>
+  </si>
+  <si>
+    <t>Misused {0} Antiviruses</t>
+  </si>
+  <si>
+    <t>Found {0} Viruses</t>
+  </si>
+  <si>
+    <t>Misused Scanner {0} Times</t>
+  </si>
+  <si>
+    <t>Used {0} Captures</t>
+  </si>
+  <si>
+    <t>Captured {0} Viruses</t>
+  </si>
+  <si>
+    <t>Misused Capture {0} Times</t>
+  </si>
+  <si>
+    <t>Used {0} Analysers</t>
+  </si>
+  <si>
+    <t>Created {0} Antiviruses</t>
+  </si>
+  <si>
+    <t>Misused Analyser {0} Times</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1032"/>
+  <dimension ref="A1:U1048"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2752,32 +2848,32 @@
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>344</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>297</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C100" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
+      <c r="B101" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C101" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B102" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="C101" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="B102" s="14" t="s">
-        <v>330</v>
       </c>
       <c r="C102" t="s">
         <v>295</v>
@@ -2785,21 +2881,21 @@
     </row>
     <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C103" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>265</v>
+      <c r="A104" s="13" t="s">
+        <v>346</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>280</v>
+        <v>347</v>
       </c>
       <c r="C104" t="s">
         <v>295</v>
@@ -2807,21 +2903,21 @@
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>332</v>
+        <v>377</v>
       </c>
       <c r="C105" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
-        <v>301</v>
+      <c r="A106" s="12" t="s">
+        <v>265</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>333</v>
+        <v>280</v>
       </c>
       <c r="C106" t="s">
         <v>295</v>
@@ -2829,10 +2925,10 @@
     </row>
     <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="C107" t="s">
         <v>295</v>
@@ -2840,10 +2936,10 @@
     </row>
     <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>302</v>
+        <v>348</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="C108" t="s">
         <v>295</v>
@@ -2851,21 +2947,21 @@
     </row>
     <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>335</v>
+        <v>378</v>
       </c>
       <c r="C109" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>267</v>
+      <c r="A110" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C110" t="s">
         <v>295</v>
@@ -2873,10 +2969,10 @@
     </row>
     <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C111" t="s">
         <v>295</v>
@@ -2884,10 +2980,10 @@
     </row>
     <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>316</v>
+        <v>350</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="C112" t="s">
         <v>295</v>
@@ -2895,21 +2991,21 @@
     </row>
     <row r="113" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>282</v>
+        <v>379</v>
       </c>
       <c r="C113" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
-        <v>304</v>
+      <c r="A114" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>338</v>
+        <v>281</v>
       </c>
       <c r="C114" t="s">
         <v>295</v>
@@ -2917,21 +3013,21 @@
     </row>
     <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C115" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="12" t="s">
-        <v>269</v>
+      <c r="A116" s="13" t="s">
+        <v>352</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>283</v>
+        <v>353</v>
       </c>
       <c r="C116" t="s">
         <v>295</v>
@@ -2939,10 +3035,10 @@
     </row>
     <row r="117" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="C117" t="s">
         <v>295</v>
@@ -2950,21 +3046,21 @@
     </row>
     <row r="118" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>341</v>
+        <v>282</v>
       </c>
       <c r="C118" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
-        <v>270</v>
+      <c r="A119" s="13" t="s">
+        <v>304</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>284</v>
+        <v>333</v>
       </c>
       <c r="C119" t="s">
         <v>295</v>
@@ -2972,10 +3068,10 @@
     </row>
     <row r="120" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="C120" t="s">
         <v>295</v>
@@ -2983,21 +3079,21 @@
     </row>
     <row r="121" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>343</v>
+        <v>381</v>
       </c>
       <c r="C121" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
-        <v>286</v>
+      <c r="A122" s="12" t="s">
+        <v>269</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C122" t="s">
         <v>295</v>
@@ -3005,10 +3101,10 @@
     </row>
     <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C123" t="s">
         <v>295</v>
@@ -3016,32 +3112,32 @@
     </row>
     <row r="124" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="C124" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="12" t="s">
-        <v>271</v>
+      <c r="A125" s="13" t="s">
+        <v>318</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>287</v>
+        <v>382</v>
       </c>
       <c r="C125" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="13" t="s">
-        <v>308</v>
+      <c r="A126" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>346</v>
+        <v>284</v>
       </c>
       <c r="C126" t="s">
         <v>295</v>
@@ -3049,21 +3145,21 @@
     </row>
     <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="C127" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>272</v>
+      <c r="A128" s="13" t="s">
+        <v>358</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>289</v>
+        <v>359</v>
       </c>
       <c r="C128" t="s">
         <v>295</v>
@@ -3071,10 +3167,10 @@
     </row>
     <row r="129" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="C129" t="s">
         <v>295</v>
@@ -3082,21 +3178,21 @@
     </row>
     <row r="130" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>349</v>
+        <v>285</v>
       </c>
       <c r="C130" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>273</v>
+      <c r="A131" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>290</v>
+        <v>336</v>
       </c>
       <c r="C131" t="s">
         <v>295</v>
@@ -3104,10 +3200,10 @@
     </row>
     <row r="132" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>310</v>
+        <v>360</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="C132" t="s">
         <v>295</v>
@@ -3115,10 +3211,10 @@
     </row>
     <row r="133" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>351</v>
+        <v>384</v>
       </c>
       <c r="C133" t="s">
         <v>295</v>
@@ -3126,10 +3222,10 @@
     </row>
     <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C134" t="s">
         <v>295</v>
@@ -3137,10 +3233,10 @@
     </row>
     <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="C135" t="s">
         <v>295</v>
@@ -3148,32 +3244,32 @@
     </row>
     <row r="136" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>324</v>
+        <v>362</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="C136" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="12" t="s">
-        <v>275</v>
+      <c r="A137" s="13" t="s">
+        <v>321</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>291</v>
+        <v>385</v>
       </c>
       <c r="C137" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="13" t="s">
-        <v>312</v>
+      <c r="A138" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="C138" t="s">
         <v>295</v>
@@ -3181,21 +3277,21 @@
     </row>
     <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C139" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="12" t="s">
-        <v>276</v>
+      <c r="A140" s="13" t="s">
+        <v>363</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>292</v>
+        <v>364</v>
       </c>
       <c r="C140" t="s">
         <v>295</v>
@@ -3203,21 +3299,21 @@
     </row>
     <row r="141" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="C141" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
-        <v>326</v>
+      <c r="A142" s="12" t="s">
+        <v>273</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>356</v>
+        <v>290</v>
       </c>
       <c r="C142" t="s">
         <v>295</v>
@@ -3225,10 +3321,10 @@
     </row>
     <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>293</v>
+        <v>339</v>
       </c>
       <c r="C143" t="s">
         <v>295</v>
@@ -3236,10 +3332,10 @@
     </row>
     <row r="144" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>314</v>
+        <v>365</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C144" t="s">
         <v>295</v>
@@ -3247,106 +3343,234 @@
     </row>
     <row r="145" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="C145" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C146" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="C147" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C148" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A149" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C149" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C150" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="C151" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A152" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C152" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C153" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C154" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C155" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="C156" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B157" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C157" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C158" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="C159" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C160" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="B145" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="C145" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="12"/>
-    </row>
-    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
-    </row>
-    <row r="148" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="12"/>
-    </row>
-    <row r="149" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="12"/>
-    </row>
-    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A150" s="12"/>
-    </row>
-    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="12"/>
-    </row>
-    <row r="152" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="12"/>
-    </row>
-    <row r="153" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A153" s="12"/>
-    </row>
-    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="12"/>
-    </row>
-    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="12"/>
-    </row>
-    <row r="156" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A156" s="12"/>
-    </row>
-    <row r="157" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A157" s="12"/>
-    </row>
-    <row r="158" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A158" s="12"/>
-    </row>
-    <row r="159" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
-    </row>
-    <row r="160" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A160" s="12"/>
-    </row>
-    <row r="161" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="12"/>
-    </row>
-    <row r="162" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B161" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C161" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
     </row>
-    <row r="163" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
     </row>
-    <row r="164" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
     </row>
-    <row r="165" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
     </row>
-    <row r="166" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
     </row>
-    <row r="167" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
     </row>
-    <row r="168" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
     </row>
-    <row r="169" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
     </row>
-    <row r="170" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
     </row>
-    <row r="171" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
     </row>
-    <row r="172" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
     </row>
-    <row r="173" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
     </row>
-    <row r="174" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
     </row>
-    <row r="175" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
     </row>
-    <row r="176" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
     </row>
     <row r="177" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
@@ -5916,6 +6140,54 @@
     </row>
     <row r="1032" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1032" s="12"/>
+    </row>
+    <row r="1033" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1033" s="12"/>
+    </row>
+    <row r="1034" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1034" s="12"/>
+    </row>
+    <row r="1035" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1035" s="12"/>
+    </row>
+    <row r="1036" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1036" s="12"/>
+    </row>
+    <row r="1037" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1037" s="12"/>
+    </row>
+    <row r="1038" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1038" s="12"/>
+    </row>
+    <row r="1039" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1039" s="12"/>
+    </row>
+    <row r="1040" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1040" s="12"/>
+    </row>
+    <row r="1041" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1041" s="12"/>
+    </row>
+    <row r="1042" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1042" s="12"/>
+    </row>
+    <row r="1043" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1043" s="12"/>
+    </row>
+    <row r="1044" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1044" s="12"/>
+    </row>
+    <row r="1045" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1045" s="12"/>
+    </row>
+    <row r="1046" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1046" s="12"/>
+    </row>
+    <row r="1047" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1047" s="12"/>
+    </row>
+    <row r="1048" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1048" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set title for summary to system report
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="394">
   <si>
     <t>Key</t>
   </si>
@@ -1195,6 +1195,12 @@
   </si>
   <si>
     <t>Misused Analyser {0} Times</t>
+  </si>
+  <si>
+    <t>SYSTEM_REPORT_TITLE</t>
+  </si>
+  <si>
+    <t>System Report</t>
   </si>
 </sst>
 </file>
@@ -1600,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1048"/>
+  <dimension ref="A1:U1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2814,22 +2820,22 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B98" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C97" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>263</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>277</v>
       </c>
       <c r="C98" t="s">
         <v>295</v>
@@ -2837,10 +2843,10 @@
     </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>328</v>
+        <v>277</v>
       </c>
       <c r="C99" t="s">
         <v>295</v>
@@ -2848,10 +2854,10 @@
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>344</v>
+        <v>296</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C100" t="s">
         <v>295</v>
@@ -2859,32 +2865,32 @@
     </row>
     <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>344</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C101" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>297</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B102" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="C101" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
+      <c r="C102" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B103" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="C102" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>329</v>
       </c>
       <c r="C103" t="s">
         <v>295</v>
@@ -2892,10 +2898,10 @@
     </row>
     <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="C104" t="s">
         <v>295</v>
@@ -2903,32 +2909,32 @@
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C105" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B106" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="C105" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
+      <c r="C106" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B107" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="C106" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B107" s="14" t="s">
-        <v>330</v>
       </c>
       <c r="C107" t="s">
         <v>295</v>
@@ -2936,10 +2942,10 @@
     </row>
     <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="C108" t="s">
         <v>295</v>
@@ -2947,10 +2953,10 @@
     </row>
     <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>301</v>
+        <v>348</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="C109" t="s">
         <v>295</v>
@@ -2958,10 +2964,10 @@
     </row>
     <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>266</v>
+        <v>301</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>279</v>
+        <v>378</v>
       </c>
       <c r="C110" t="s">
         <v>295</v>
@@ -2969,10 +2975,10 @@
     </row>
     <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>331</v>
+        <v>279</v>
       </c>
       <c r="C111" t="s">
         <v>295</v>
@@ -2980,10 +2986,10 @@
     </row>
     <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C112" t="s">
         <v>295</v>
@@ -2991,32 +2997,32 @@
     </row>
     <row r="113" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C113" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B114" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="C113" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
+      <c r="C114" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B115" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="C114" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>332</v>
       </c>
       <c r="C115" t="s">
         <v>295</v>
@@ -3024,10 +3030,10 @@
     </row>
     <row r="116" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>352</v>
+        <v>303</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="C116" t="s">
         <v>295</v>
@@ -3035,10 +3041,10 @@
     </row>
     <row r="117" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="C117" t="s">
         <v>295</v>
@@ -3046,10 +3052,10 @@
     </row>
     <row r="118" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>268</v>
+        <v>316</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>282</v>
+        <v>380</v>
       </c>
       <c r="C118" t="s">
         <v>295</v>
@@ -3057,10 +3063,10 @@
     </row>
     <row r="119" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>333</v>
+        <v>282</v>
       </c>
       <c r="C119" t="s">
         <v>295</v>
@@ -3068,10 +3074,10 @@
     </row>
     <row r="120" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C120" t="s">
         <v>295</v>
@@ -3079,32 +3085,32 @@
     </row>
     <row r="121" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C121" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="B121" s="14" t="s">
+      <c r="B122" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="C121" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="12" t="s">
+      <c r="C122" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B123" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="C122" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>334</v>
       </c>
       <c r="C123" t="s">
         <v>295</v>
@@ -3112,10 +3118,10 @@
     </row>
     <row r="124" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>356</v>
+        <v>305</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="C124" t="s">
         <v>295</v>
@@ -3123,32 +3129,32 @@
     </row>
     <row r="125" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C125" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="B125" s="14" t="s">
+      <c r="B126" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="C125" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
+      <c r="C126" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B127" s="14" t="s">
         <v>284</v>
-      </c>
-      <c r="C126" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>335</v>
       </c>
       <c r="C127" t="s">
         <v>295</v>
@@ -3156,10 +3162,10 @@
     </row>
     <row r="128" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>358</v>
+        <v>306</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="C128" t="s">
         <v>295</v>
@@ -3167,10 +3173,10 @@
     </row>
     <row r="129" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="C129" t="s">
         <v>295</v>
@@ -3178,10 +3184,10 @@
     </row>
     <row r="130" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>286</v>
+        <v>319</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>285</v>
+        <v>383</v>
       </c>
       <c r="C130" t="s">
         <v>295</v>
@@ -3189,10 +3195,10 @@
     </row>
     <row r="131" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>336</v>
+        <v>285</v>
       </c>
       <c r="C131" t="s">
         <v>295</v>
@@ -3200,10 +3206,10 @@
     </row>
     <row r="132" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>360</v>
+        <v>307</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="C132" t="s">
         <v>295</v>
@@ -3211,32 +3217,32 @@
     </row>
     <row r="133" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C133" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="B133" s="14" t="s">
+      <c r="B134" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="C133" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="12" t="s">
+      <c r="C134" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B135" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="C134" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>337</v>
       </c>
       <c r="C135" t="s">
         <v>295</v>
@@ -3244,10 +3250,10 @@
     </row>
     <row r="136" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>362</v>
+        <v>308</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="C136" t="s">
         <v>295</v>
@@ -3255,32 +3261,32 @@
     </row>
     <row r="137" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C137" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="B137" s="14" t="s">
+      <c r="B138" s="14" t="s">
         <v>385</v>
       </c>
-      <c r="C137" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="12" t="s">
+      <c r="C138" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="B138" s="14" t="s">
+      <c r="B139" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="C138" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>338</v>
       </c>
       <c r="C139" t="s">
         <v>295</v>
@@ -3288,10 +3294,10 @@
     </row>
     <row r="140" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
-        <v>363</v>
+        <v>309</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="C140" t="s">
         <v>295</v>
@@ -3299,32 +3305,32 @@
     </row>
     <row r="141" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C141" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="B141" s="14" t="s">
+      <c r="B142" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="C141" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="12" t="s">
+      <c r="C142" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B143" s="14" t="s">
         <v>290</v>
-      </c>
-      <c r="C142" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>339</v>
       </c>
       <c r="C143" t="s">
         <v>295</v>
@@ -3332,10 +3338,10 @@
     </row>
     <row r="144" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>365</v>
+        <v>310</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="C144" t="s">
         <v>295</v>
@@ -3343,32 +3349,32 @@
     </row>
     <row r="145" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C145" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="B145" s="14" t="s">
+      <c r="B146" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="C145" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="12" t="s">
+      <c r="C146" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B147" s="14" t="s">
         <v>288</v>
-      </c>
-      <c r="C146" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A147" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B147" s="14" t="s">
-        <v>340</v>
       </c>
       <c r="C147" t="s">
         <v>295</v>
@@ -3376,10 +3382,10 @@
     </row>
     <row r="148" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
-        <v>367</v>
+        <v>311</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
       <c r="C148" t="s">
         <v>295</v>
@@ -3387,32 +3393,32 @@
     </row>
     <row r="149" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C149" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="B149" s="14" t="s">
+      <c r="B150" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="C149" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A150" s="12" t="s">
+      <c r="C150" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B150" s="14" t="s">
+      <c r="B151" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="C150" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="B151" s="14" t="s">
-        <v>341</v>
       </c>
       <c r="C151" t="s">
         <v>295</v>
@@ -3420,10 +3426,10 @@
     </row>
     <row r="152" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
-        <v>368</v>
+        <v>312</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
       <c r="C152" t="s">
         <v>295</v>
@@ -3431,32 +3437,32 @@
     </row>
     <row r="153" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C153" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="B153" s="14" t="s">
+      <c r="B154" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="C153" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="12" t="s">
+      <c r="C154" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B155" s="14" t="s">
         <v>292</v>
-      </c>
-      <c r="C154" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B155" s="14" t="s">
-        <v>342</v>
       </c>
       <c r="C155" t="s">
         <v>295</v>
@@ -3464,10 +3470,10 @@
     </row>
     <row r="156" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
-        <v>370</v>
+        <v>313</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="C156" t="s">
         <v>295</v>
@@ -3475,10 +3481,10 @@
     </row>
     <row r="157" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
-        <v>326</v>
+        <v>370</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="C157" t="s">
         <v>295</v>
@@ -3486,10 +3492,10 @@
     </row>
     <row r="158" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>293</v>
+        <v>390</v>
       </c>
       <c r="C158" t="s">
         <v>295</v>
@@ -3497,10 +3503,10 @@
     </row>
     <row r="159" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
       <c r="C159" t="s">
         <v>295</v>
@@ -3508,10 +3514,10 @@
     </row>
     <row r="160" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>372</v>
+        <v>314</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>373</v>
+        <v>343</v>
       </c>
       <c r="C160" t="s">
         <v>295</v>
@@ -3519,17 +3525,25 @@
     </row>
     <row r="161" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C161" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="B161" s="14" t="s">
+      <c r="B162" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="C161" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A162" s="12"/>
+      <c r="C162" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="163" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
@@ -6188,6 +6202,9 @@
     </row>
     <row r="1048" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1048" s="12"/>
+    </row>
+    <row r="1049" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1049" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update localizations to replace colour with icon
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -288,12 +288,6 @@
     <t>LOBBY_BUTTON_COLOUR</t>
   </si>
   <si>
-    <t>Change Colour</t>
-  </si>
-  <si>
-    <t>Verander Kleur</t>
-  </si>
-  <si>
     <t>LOBBY_BUTTON_READY</t>
   </si>
   <si>
@@ -400,12 +394,6 @@
   </si>
   <si>
     <t>COLOUR_PICKER_LABEL_TITLE</t>
-  </si>
-  <si>
-    <t>Change Player Colour</t>
-  </si>
-  <si>
-    <t>Verander Kleur Speler</t>
   </si>
   <si>
     <t>COLOUR_PICKER_BUTTON_CANCEL</t>
@@ -1220,13 +1208,25 @@
   </si>
   <si>
     <t>Final Score</t>
+  </si>
+  <si>
+    <t>Change Icon</t>
+  </si>
+  <si>
+    <t>Verander Icoon</t>
+  </si>
+  <si>
+    <t>Change Player Icon</t>
+  </si>
+  <si>
+    <t>Verander Icoon Speler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1245,8 +1245,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1257,6 +1264,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1298,10 +1310,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1324,8 +1337,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1630,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2146,15 +2161,15 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>90</v>
+        <v>396</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>397</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -2162,13 +2177,13 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2176,13 +2191,13 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2190,13 +2205,13 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2204,13 +2219,13 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2218,13 +2233,13 @@
     </row>
     <row r="41" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2232,13 +2247,13 @@
     </row>
     <row r="42" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2246,13 +2261,13 @@
     </row>
     <row r="43" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2260,18 +2275,18 @@
     </row>
     <row r="44" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>62</v>
@@ -2282,348 +2297,348 @@
     </row>
     <row r="46" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>128</v>
+      <c r="B50" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>62</v>
@@ -2634,970 +2649,970 @@
     </row>
     <row r="78" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C84" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C85" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C86" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C87" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C88" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C89" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C90" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C91" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C92" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C93" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C94" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C95" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="C96" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C96" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A97" s="13" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C97" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>259</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>291</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C100" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>339</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C101" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>292</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C103" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C104" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C105" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C107" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C108" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C113" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C116" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A117" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C119" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A120" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A121" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C121" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A122" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C123" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C125" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A129" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A130" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A131" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C131" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A132" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C133" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A135" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A136" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="C136" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C137" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C138" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A139" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C139" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A140" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C140" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C141" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A142" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C142" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C144" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A145" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C145" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A147" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C147" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A148" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C148" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C149" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A151" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A152" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A153" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C153" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A154" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C154" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C155" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C156" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A157" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="B157" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A159" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C159" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A160" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C160" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A161" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A162" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C162" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A164" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="B164" s="14" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>263</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C99" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>295</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C100" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>343</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="C101" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>296</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="C102" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C103" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="B104" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="C104" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="B105" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="C105" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="B106" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="C106" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="B107" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C107" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="C108" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="C109" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B110" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="C110" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C111" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="C112" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="C113" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B114" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="C114" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="C115" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="C116" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="B117" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="C117" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="B118" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="C118" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="C119" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="B120" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="C120" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="C121" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="B122" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="C122" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C123" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B124" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="C124" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="C125" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B126" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="C126" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="C127" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="B128" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="C128" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="B129" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="C129" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="B130" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="C130" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="C131" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B132" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="C132" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="C133" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B134" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="C134" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C135" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="C136" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B137" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="C137" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="B138" s="14" t="s">
-        <v>384</v>
-      </c>
-      <c r="C138" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="C139" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="C140" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="B141" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="C141" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="B142" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="C142" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="C143" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A144" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="B144" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="C144" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="B145" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="C145" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="B146" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="C146" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A147" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B147" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="C147" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="B148" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="C148" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="B149" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="C149" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A150" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="B150" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="C150" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="B151" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="C151" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B152" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="C152" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A153" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="B153" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="C153" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B154" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="C154" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="B155" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="C155" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A156" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="B156" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="C156" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A157" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="B157" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="C157" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A158" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="B158" s="14" t="s">
-        <v>389</v>
-      </c>
-      <c r="C158" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A159" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="B159" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="C159" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A160" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B160" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="C160" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="B161" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="C161" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A162" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="B162" s="14" t="s">
-        <v>390</v>
-      </c>
-      <c r="C162" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A163" s="13" t="s">
+      <c r="C164" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A165" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="B163" s="15" t="s">
+      <c r="B165" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="C163" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A164" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="B164" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="C164" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A165" s="13" t="s">
-        <v>397</v>
-      </c>
-      <c r="B165" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="C165" t="s">
-        <v>394</v>
+      <c r="C165" s="16" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
press here to talk for mobile localization added
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\ITALERTTEST\Unity\Assets\Editor\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\it-alert\Unity\Assets\Editor\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{34338979-2E37-4881-8A10-0FF33431DD2B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UILocalizations" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="403">
   <si>
     <t>Key</t>
   </si>
@@ -1220,12 +1221,21 @@
   </si>
   <si>
     <t>Verander Icoon Speler</t>
+  </si>
+  <si>
+    <t>VOICE_PRESS_TO_TALK</t>
+  </si>
+  <si>
+    <t>Druk hier om te praten</t>
+  </si>
+  <si>
+    <t>Press here to talk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1432,6 +1442,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1467,6 +1494,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1642,11 +1686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1049"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2078,14 +2122,14 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>73</v>
+      <c r="A30" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>401</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2093,27 +2137,27 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>77</v>
+      <c r="A32" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -2121,27 +2165,27 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>83</v>
+      <c r="A34" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -2149,41 +2193,41 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>397</v>
+        <v>86</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>91</v>
+        <v>396</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>397</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2191,13 +2235,13 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2205,13 +2249,13 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2219,27 +2263,27 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2247,13 +2291,13 @@
     </row>
     <row r="42" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2261,13 +2305,13 @@
     </row>
     <row r="43" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2275,615 +2319,618 @@
     </row>
     <row r="44" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B45" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>115</v>
+        <v>62</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B50" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C51" s="16" t="s">
         <v>399</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C77" s="9" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="78" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+    <row r="79" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C79" s="9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+    <row r="80" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B80" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C84" t="s">
-        <v>243</v>
+        <v>220</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C85" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C88" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C89" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C90" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C91" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C92" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C94" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C95" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B96" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="12" t="s">
+    <row r="97" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B97" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C96" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="13" t="s">
+      <c r="C97" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B98" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C97" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="12" t="s">
+      <c r="C98" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="B99" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C98" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>259</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="C99" s="16" t="s">
         <v>390</v>
@@ -2891,10 +2938,10 @@
     </row>
     <row r="100" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="C100" s="16" t="s">
         <v>390</v>
@@ -2902,10 +2949,10 @@
     </row>
     <row r="101" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="C101" s="16" t="s">
         <v>390</v>
@@ -2913,32 +2960,32 @@
     </row>
     <row r="102" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>339</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>292</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B103" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C102" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="12" t="s">
+      <c r="C103" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B104" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="C103" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="B104" s="14" t="s">
-        <v>324</v>
       </c>
       <c r="C104" s="16" t="s">
         <v>390</v>
@@ -2946,10 +2993,10 @@
     </row>
     <row r="105" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A105" s="13" t="s">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>390</v>
@@ -2957,32 +3004,32 @@
     </row>
     <row r="106" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A106" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B107" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="C106" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="12" t="s">
+      <c r="C107" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B108" s="14" t="s">
         <v>276</v>
-      </c>
-      <c r="C107" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>325</v>
       </c>
       <c r="C108" s="16" t="s">
         <v>390</v>
@@ -2990,10 +3037,10 @@
     </row>
     <row r="109" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A109" s="13" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>390</v>
@@ -3001,10 +3048,10 @@
     </row>
     <row r="110" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A110" s="13" t="s">
-        <v>296</v>
+        <v>343</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="C110" s="16" t="s">
         <v>390</v>
@@ -3012,10 +3059,10 @@
     </row>
     <row r="111" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A111" s="13" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>275</v>
+        <v>373</v>
       </c>
       <c r="C111" s="16" t="s">
         <v>390</v>
@@ -3023,10 +3070,10 @@
     </row>
     <row r="112" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A112" s="13" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="C112" s="16" t="s">
         <v>390</v>
@@ -3034,10 +3081,10 @@
     </row>
     <row r="113" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A113" s="13" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C113" s="16" t="s">
         <v>390</v>
@@ -3045,32 +3092,32 @@
     </row>
     <row r="114" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A114" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B115" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="C114" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="12" t="s">
+      <c r="C115" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B116" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="C115" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>327</v>
       </c>
       <c r="C116" s="16" t="s">
         <v>390</v>
@@ -3078,10 +3125,10 @@
     </row>
     <row r="117" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="13" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C117" s="16" t="s">
         <v>390</v>
@@ -3089,10 +3136,10 @@
     </row>
     <row r="118" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
-        <v>311</v>
+        <v>347</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="C118" s="16" t="s">
         <v>390</v>
@@ -3100,10 +3147,10 @@
     </row>
     <row r="119" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A119" s="13" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>278</v>
+        <v>375</v>
       </c>
       <c r="C119" s="16" t="s">
         <v>390</v>
@@ -3111,10 +3158,10 @@
     </row>
     <row r="120" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A120" s="13" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="C120" s="16" t="s">
         <v>390</v>
@@ -3122,10 +3169,10 @@
     </row>
     <row r="121" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" s="13" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="C121" s="16" t="s">
         <v>390</v>
@@ -3133,32 +3180,32 @@
     </row>
     <row r="122" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B123" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="C122" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A123" s="12" t="s">
+      <c r="C123" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B124" s="14" t="s">
         <v>279</v>
-      </c>
-      <c r="C123" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A124" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B124" s="14" t="s">
-        <v>329</v>
       </c>
       <c r="C124" s="16" t="s">
         <v>390</v>
@@ -3166,10 +3213,10 @@
     </row>
     <row r="125" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="13" t="s">
-        <v>351</v>
+        <v>300</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="C125" s="16" t="s">
         <v>390</v>
@@ -3177,32 +3224,32 @@
     </row>
     <row r="126" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B127" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="C126" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A127" s="12" t="s">
+      <c r="C127" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="B128" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="C127" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A128" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="B128" s="14" t="s">
-        <v>330</v>
       </c>
       <c r="C128" s="16" t="s">
         <v>390</v>
@@ -3210,10 +3257,10 @@
     </row>
     <row r="129" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C129" s="16" t="s">
         <v>390</v>
@@ -3221,10 +3268,10 @@
     </row>
     <row r="130" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
-        <v>314</v>
+        <v>353</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C130" s="16" t="s">
         <v>390</v>
@@ -3232,10 +3279,10 @@
     </row>
     <row r="131" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>281</v>
+        <v>378</v>
       </c>
       <c r="C131" s="16" t="s">
         <v>390</v>
@@ -3243,10 +3290,10 @@
     </row>
     <row r="132" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="C132" s="16" t="s">
         <v>390</v>
@@ -3254,10 +3301,10 @@
     </row>
     <row r="133" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
-        <v>355</v>
+        <v>302</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="C133" s="16" t="s">
         <v>390</v>
@@ -3265,32 +3312,32 @@
     </row>
     <row r="134" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A135" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B135" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="C134" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A135" s="12" t="s">
+      <c r="C135" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A136" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="14" t="s">
+      <c r="B136" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="C135" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A136" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>332</v>
       </c>
       <c r="C136" s="16" t="s">
         <v>390</v>
@@ -3298,10 +3345,10 @@
     </row>
     <row r="137" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" s="13" t="s">
-        <v>357</v>
+        <v>303</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="C137" s="16" t="s">
         <v>390</v>
@@ -3309,32 +3356,32 @@
     </row>
     <row r="138" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C138" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A139" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="B138" s="14" t="s">
+      <c r="B139" s="14" t="s">
         <v>380</v>
       </c>
-      <c r="C138" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A139" s="12" t="s">
+      <c r="C139" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A140" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B140" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="C139" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A140" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>333</v>
       </c>
       <c r="C140" s="16" t="s">
         <v>390</v>
@@ -3342,10 +3389,10 @@
     </row>
     <row r="141" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="13" t="s">
-        <v>358</v>
+        <v>304</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="C141" s="16" t="s">
         <v>390</v>
@@ -3353,32 +3400,32 @@
     </row>
     <row r="142" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A142" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C142" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B143" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="C142" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A143" s="12" t="s">
+      <c r="C143" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="B143" s="14" t="s">
+      <c r="B144" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="B144" s="14" t="s">
-        <v>334</v>
       </c>
       <c r="C144" s="16" t="s">
         <v>390</v>
@@ -3386,10 +3433,10 @@
     </row>
     <row r="145" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A145" s="13" t="s">
-        <v>360</v>
+        <v>305</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="C145" s="16" t="s">
         <v>390</v>
@@ -3397,32 +3444,32 @@
     </row>
     <row r="146" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A146" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A147" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B147" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="C146" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A147" s="12" t="s">
+      <c r="C147" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A148" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B147" s="14" t="s">
+      <c r="B148" s="14" t="s">
         <v>284</v>
-      </c>
-      <c r="C147" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B148" s="14" t="s">
-        <v>335</v>
       </c>
       <c r="C148" s="16" t="s">
         <v>390</v>
@@ -3430,10 +3477,10 @@
     </row>
     <row r="149" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A149" s="13" t="s">
-        <v>362</v>
+        <v>306</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="C149" s="16" t="s">
         <v>390</v>
@@ -3441,32 +3488,32 @@
     </row>
     <row r="150" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A150" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A151" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="B150" s="14" t="s">
+      <c r="B151" s="14" t="s">
         <v>383</v>
       </c>
-      <c r="C150" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="12" t="s">
+      <c r="C151" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A152" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="B151" s="14" t="s">
+      <c r="B152" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="C151" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A152" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="B152" s="14" t="s">
-        <v>336</v>
       </c>
       <c r="C152" s="16" t="s">
         <v>390</v>
@@ -3474,10 +3521,10 @@
     </row>
     <row r="153" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A153" s="13" t="s">
-        <v>363</v>
+        <v>307</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
       <c r="C153" s="16" t="s">
         <v>390</v>
@@ -3485,32 +3532,32 @@
     </row>
     <row r="154" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A154" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C154" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B155" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="C154" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A155" s="12" t="s">
+      <c r="C155" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="B155" s="14" t="s">
+      <c r="B156" s="14" t="s">
         <v>288</v>
-      </c>
-      <c r="C155" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A156" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B156" s="14" t="s">
-        <v>337</v>
       </c>
       <c r="C156" s="16" t="s">
         <v>390</v>
@@ -3518,10 +3565,10 @@
     </row>
     <row r="157" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="13" t="s">
-        <v>365</v>
+        <v>308</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="C157" s="16" t="s">
         <v>390</v>
@@ -3529,10 +3576,10 @@
     </row>
     <row r="158" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" s="13" t="s">
-        <v>321</v>
+        <v>365</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="C158" s="16" t="s">
         <v>390</v>
@@ -3540,10 +3587,10 @@
     </row>
     <row r="159" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" s="13" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>289</v>
+        <v>385</v>
       </c>
       <c r="C159" s="16" t="s">
         <v>390</v>
@@ -3551,10 +3598,10 @@
     </row>
     <row r="160" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" s="13" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="C160" s="16" t="s">
         <v>390</v>
@@ -3562,10 +3609,10 @@
     </row>
     <row r="161" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" s="13" t="s">
-        <v>367</v>
+        <v>309</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>368</v>
+        <v>338</v>
       </c>
       <c r="C161" s="16" t="s">
         <v>390</v>
@@ -3573,32 +3620,32 @@
     </row>
     <row r="162" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C162" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="B162" s="14" t="s">
+      <c r="B163" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="C162" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="38.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="13" t="s">
+      <c r="C163" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A164" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="B163" s="15" t="s">
+      <c r="B164" s="15" t="s">
         <v>391</v>
-      </c>
-      <c r="C163" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A164" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="B164" s="14" t="s">
-        <v>394</v>
       </c>
       <c r="C164" s="16" t="s">
         <v>390</v>
@@ -3606,17 +3653,25 @@
     </row>
     <row r="165" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A165" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C165" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A166" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="B165" s="14" t="s">
+      <c r="B166" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="C165" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A166" s="12"/>
+      <c r="C166" s="16" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="167" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
@@ -6266,6 +6321,9 @@
     </row>
     <row r="1049" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1049" s="12"/>
+    </row>
+    <row r="1050" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1050" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated press to talk
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\it-alert\Unity\Assets\Editor\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{34338979-2E37-4881-8A10-0FF33431DD2B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{052D1EF8-FD3B-4F79-91DB-989A28BA1B39}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,10 +1226,10 @@
     <t>VOICE_PRESS_TO_TALK</t>
   </si>
   <si>
-    <t>Druk hier om te praten</t>
-  </si>
-  <si>
-    <t>Press here to talk</t>
+    <t>Press to talk</t>
+  </si>
+  <si>
+    <t>Druk om te praten</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1690,7 @@
   <dimension ref="A1:U1050"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2126,10 +2126,10 @@
         <v>400</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>402</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>

</xml_diff>

<commit_message>
changed to "health multiplier" and fixed cutoff issue
</commit_message>
<xml_diff>
--- a/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
+++ b/Unity/Assets/Editor/Localization/IT Alert UI Translation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\it-alert\Unity\Assets\Editor\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F8739041-3A6A-4D8A-B540-ABC03F53A4FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0923A974-038B-44D0-A0B6-59C20BCBB80D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="600" windowWidth="27500" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1190,9 +1190,6 @@
     <t>GAME_OVER_FINAL_SCORE</t>
   </si>
   <si>
-    <t>Multiplier</t>
-  </si>
-  <si>
     <t>Final Score</t>
   </si>
   <si>
@@ -1230,6 +1227,9 @@
   </si>
   <si>
     <t>Druk om te praten</t>
+  </si>
+  <si>
+    <t>Health Multiplier</t>
   </si>
 </sst>
 </file>
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2123,13 +2123,13 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2221,13 +2221,13 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>391</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>392</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2399,18 +2399,18 @@
     </row>
     <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C51" s="16" t="s">
         <v>393</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>123</v>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="53" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>125</v>
@@ -3656,7 +3656,7 @@
         <v>387</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C165" s="16" t="s">
         <v>385</v>
@@ -3667,7 +3667,7 @@
         <v>388</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C166" s="16" t="s">
         <v>385</v>

</xml_diff>